<commit_message>
feat: Created directory for PROG1085
</commit_message>
<xml_diff>
--- a/Courses/PROG1500 - Databases and SQL/Modules/Final Project/Final_Project.xlsx
+++ b/Courses/PROG1500 - Databases and SQL/Modules/Final Project/Final_Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4400113921\Desktop\Ryan\Software_Technology\Courses\PROG1500 - Databases and SQL\Modules\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C934CB-D676-4102-A155-7B7510F70BE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27400EF-1E49-4B92-84A8-CC9813516570}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15480" windowHeight="9645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1150,7 +1150,7 @@
         <v>custphone</v>
       </c>
       <c r="O10" s="2" t="str">
-        <f t="shared" ref="N10:O10" si="1">LOWER(O3)</f>
+        <f t="shared" ref="O10" si="1">LOWER(O3)</f>
         <v>datepurch</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Started database design for PROG1500 Final Project
</commit_message>
<xml_diff>
--- a/Courses/PROG1500 - Databases and SQL/Modules/Final Project/Final_Project.xlsx
+++ b/Courses/PROG1500 - Databases and SQL/Modules/Final Project/Final_Project.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4400113921\Desktop\Ryan\Software_Technology\Courses\PROG1500 - Databases and SQL\Modules\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27400EF-1E49-4B92-84A8-CC9813516570}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3B6AE5-05F5-47B2-B30B-5F83EC916437}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15480" windowHeight="9645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15480" windowHeight="9645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="student" sheetId="1" r:id="rId1"/>
-    <sheet name="student_class" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Fake Online Bookstore dataset" sheetId="1" r:id="rId1"/>
+    <sheet name="author table" sheetId="2" r:id="rId2"/>
+    <sheet name="book table" sheetId="3" r:id="rId3"/>
+    <sheet name="reviewer table" sheetId="4" r:id="rId4"/>
+    <sheet name="customer table" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="87">
   <si>
     <t>PK</t>
   </si>
@@ -63,9 +65,6 @@
     <t>class_student table</t>
   </si>
   <si>
-    <t>Fake Online Bookstore</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -208,16 +207,95 @@
   </si>
   <si>
     <t>978-323-1226</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>author_id</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>book_id</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>date_reviewed</t>
+  </si>
+  <si>
+    <t>cust_email</t>
+  </si>
+  <si>
+    <t>date_purch</t>
+  </si>
+  <si>
+    <t>cust_phone</t>
+  </si>
+  <si>
+    <t>cust_adddress</t>
+  </si>
+  <si>
+    <t>cust_name</t>
+  </si>
+  <si>
+    <t>author_1</t>
+  </si>
+  <si>
+    <t>author_2</t>
+  </si>
+  <si>
+    <t>author_3</t>
+  </si>
+  <si>
+    <t>Fake Online Bookstore dataset</t>
+  </si>
+  <si>
+    <t>book table</t>
+  </si>
+  <si>
+    <t>Tony</t>
+  </si>
+  <si>
+    <t>Gaddis</t>
+  </si>
+  <si>
+    <t>Muganda</t>
+  </si>
+  <si>
+    <t>middle_name</t>
+  </si>
+  <si>
+    <t>Niederst</t>
+  </si>
+  <si>
+    <t>Robbins</t>
+  </si>
+  <si>
+    <t>Ullman</t>
+  </si>
+  <si>
+    <t>Walters</t>
+  </si>
+  <si>
+    <t>Godfrey</t>
+  </si>
+  <si>
+    <t>Jennifer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="166" formatCode="0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,8 +340,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,8 +371,19 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -433,14 +530,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -455,12 +596,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -486,7 +621,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -510,9 +644,45 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="6" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="4"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
@@ -851,435 +1021,543 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:O42"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" style="26" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" style="23" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="65.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" customWidth="1"/>
     <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
+    <row r="1" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="38" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="19" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="20">
+        <v>100</v>
+      </c>
+      <c r="G4" s="25">
+        <v>132855836</v>
+      </c>
+      <c r="H4" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="23">
+      <c r="I4" s="21">
+        <v>41416</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="21">
+        <v>41958</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="20">
+        <v>109</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="21">
+        <v>41416</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" s="21">
+        <v>41991</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20">
+        <v>27</v>
+      </c>
+      <c r="G6" s="25">
+        <v>321784073</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="21">
+        <v>41416</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="M6" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="O6" s="21">
+        <v>41654</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="20">
+        <v>34</v>
+      </c>
+      <c r="G7" s="25">
+        <v>1449319270</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="21">
+        <v>41416</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="L7" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="M7" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="N7" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="O7" s="21">
+        <v>41867</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="42"/>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="2" t="str">
+        <f>LOWER(F3)</f>
+        <v>price</v>
+      </c>
+      <c r="G12" s="26" t="str">
+        <f>LOWER(G3)</f>
+        <v>isbn</v>
+      </c>
+      <c r="H12" s="2" t="str">
+        <f>LOWER(H3)</f>
+        <v>reviewer</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J12" s="2" t="str">
+        <f>LOWER(J3)</f>
+        <v>review</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="30">
+        <v>1</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32">
         <v>100</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G13" s="33">
         <v>132855836</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H13" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="34">
+        <v>41416</v>
+      </c>
+      <c r="J13" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="24">
+      <c r="K13" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="M13" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="O13" s="34">
+        <v>41958</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="30">
+        <v>2</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="32">
+        <v>109</v>
+      </c>
+      <c r="G14" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="34">
         <v>41416</v>
       </c>
-      <c r="J4" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="M4" s="25" t="s">
+      <c r="J14" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K14" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="L14" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="M14" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="N14" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="O14" s="34">
+        <v>41991</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="30">
+        <v>3</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32">
+        <v>27</v>
+      </c>
+      <c r="G15" s="33">
+        <v>321784073</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="34">
+        <v>41416</v>
+      </c>
+      <c r="J15" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="L15" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="M15" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="N15" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="O15" s="34">
+        <v>41654</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="30">
+        <v>4</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="32">
         <v>34</v>
       </c>
-      <c r="N4" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="O4" s="24">
-        <v>41958</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="23">
-        <v>109</v>
-      </c>
-      <c r="G5" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="24">
+      <c r="G16" s="33">
+        <v>1449319270</v>
+      </c>
+      <c r="H16" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="34">
         <v>41416</v>
       </c>
-      <c r="J5" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="K5" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="M5" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="N5" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="O5" s="24">
-        <v>41991</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="23">
-        <v>27</v>
-      </c>
-      <c r="G6" s="28">
-        <v>321784073</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="I6" s="24">
-        <v>41416</v>
-      </c>
-      <c r="J6" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="K6" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="L6" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="M6" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="N6" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="O6" s="24">
-        <v>41654</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="23">
-        <v>34</v>
-      </c>
-      <c r="G7" s="28">
-        <v>1449319270</v>
-      </c>
-      <c r="H7" s="22" t="s">
+      <c r="J16" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="24">
-        <v>41416</v>
-      </c>
-      <c r="J7" s="24" t="s">
+      <c r="K16" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="L16" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="L7" s="22" t="s">
+      <c r="M16" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="M7" s="25" t="s">
+      <c r="N16" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="N7" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="O7" s="24">
+      <c r="O16" s="34">
         <v>41867</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F17" s="23"/>
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="18"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="H9" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="str">
-        <f t="shared" ref="B10:M10" si="0">LOWER(B3)</f>
+      <c r="I19" s="18"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="str">
+        <f>LOWER(B12)</f>
         <v>title</v>
       </c>
-      <c r="C10" s="2" t="str">
+      <c r="C20" s="2" t="str">
+        <f t="shared" ref="C20:E20" si="0">LOWER(C12)</f>
+        <v>author_1</v>
+      </c>
+      <c r="D20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>author1</v>
-      </c>
-      <c r="D10" s="2" t="str">
+        <v>author_2</v>
+      </c>
+      <c r="E20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>author2</v>
-      </c>
-      <c r="E10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>author3</v>
-      </c>
-      <c r="F10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>price</v>
-      </c>
-      <c r="G10" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>isbn</v>
-      </c>
-      <c r="H10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>reviewer</v>
-      </c>
-      <c r="I10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>datereviewed</v>
-      </c>
-      <c r="J10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>review</v>
-      </c>
-      <c r="K10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>custemail</v>
-      </c>
-      <c r="L10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>custname</v>
-      </c>
-      <c r="M10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>custaddress</v>
-      </c>
-      <c r="N10" s="2" t="str">
-        <f>LOWER(N3)</f>
-        <v>custphone</v>
-      </c>
-      <c r="O10" s="2" t="str">
-        <f t="shared" ref="O10" si="1">LOWER(O3)</f>
-        <v>datepurch</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="6"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="6"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="6"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="6"/>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="20"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="I17" s="20"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="str">
-        <f>LOWER(B10)</f>
-        <v>title</v>
-      </c>
-      <c r="C18" s="2" t="str">
-        <f t="shared" ref="C18:E18" si="2">LOWER(C10)</f>
-        <v>author1</v>
-      </c>
-      <c r="D18" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>author2</v>
-      </c>
-      <c r="E18" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>author3</v>
-      </c>
-      <c r="F18" s="2" t="s">
+        <v>author_3</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="29" t="s">
+      <c r="G20" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="2"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
@@ -1287,7 +1565,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="29"/>
+      <c r="G21" s="26"/>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -1296,101 +1574,109 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="29"/>
+      <c r="G22" s="26"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="10" t="s">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="13" t="s">
+      <c r="C27" s="6"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C28" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D26" s="18"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="15" t="s">
+      <c r="D28" s="16"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C29" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="19"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
+      <c r="D29" s="17"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="11"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="12"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="4"/>
+      <c r="E31" s="9"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="10" t="s">
+      <c r="D32" s="10"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="16" t="s">
+      <c r="C37" s="6"/>
+      <c r="D37" s="7"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D36" s="17"/>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
+      <c r="D38" s="15"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="3"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="3"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
@@ -1403,7 +1689,17 @@
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F42" s="11"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="3"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F44" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1413,13 +1709,131 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A3:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="28">
+        <v>1</v>
+      </c>
+      <c r="C4" s="28">
+        <v>1</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="28">
+        <v>1</v>
+      </c>
+      <c r="C5" s="28">
+        <v>2</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="28">
+        <v>2</v>
+      </c>
+      <c r="C6" s="28">
+        <v>2</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="28">
+        <v>3</v>
+      </c>
+      <c r="C7" s="28">
+        <v>4</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="28">
+        <v>4</v>
+      </c>
+      <c r="C8" s="28">
+        <v>3</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="28">
+        <v>5</v>
+      </c>
+      <c r="C9" s="28">
+        <v>2</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1433,4 +1847,28 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E15CAA-4777-4BDE-A5C1-09049BF5293E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A6F80E-60BB-4B9E-9A06-656EDAEA79F7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Completed book and reviewer tables for PROG1500 Final
</commit_message>
<xml_diff>
--- a/Courses/PROG1500 - Databases and SQL/Modules/Final Project/Final_Project.xlsx
+++ b/Courses/PROG1500 - Databases and SQL/Modules/Final Project/Final_Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4400113921\Desktop\Ryan\Software_Technology\Courses\PROG1500 - Databases and SQL\Modules\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3B6AE5-05F5-47B2-B30B-5F83EC916437}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900D97C7-7D25-42D3-9B1B-2CB662E7EA41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15480" windowHeight="9645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15480" windowHeight="9645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fake Online Bookstore dataset" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="109">
   <si>
     <t>PK</t>
   </si>
@@ -285,6 +285,72 @@
   </si>
   <si>
     <t>Jennifer</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>isbn</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>reviewer</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>reviewer_id</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Justin</t>
+  </si>
+  <si>
+    <t>Melissa</t>
+  </si>
+  <si>
+    <t>Zack</t>
+  </si>
+  <si>
+    <t>Skyler</t>
+  </si>
+  <si>
+    <t>Steff</t>
+  </si>
+  <si>
+    <t>"Good book"</t>
+  </si>
+  <si>
+    <t>"Excellent Book to Learn Java"</t>
+  </si>
+  <si>
+    <t>"Good reference book"</t>
+  </si>
+  <si>
+    <t>"EXCELLENT"</t>
+  </si>
+  <si>
+    <t>"best hands-on book for C++"</t>
+  </si>
+  <si>
+    <t>"For me; unusable"</t>
+  </si>
+  <si>
+    <t>"Its the book you need if you want to learn HTML"</t>
   </si>
 </sst>
 </file>
@@ -293,9 +359,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="166" formatCode="0000"/>
+    <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,8 +414,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,6 +455,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -574,14 +652,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -644,11 +723,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
@@ -666,7 +742,7 @@
     <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
@@ -679,10 +755,30 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
+    <cellStyle name="Good" xfId="5" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
@@ -1024,7 +1120,7 @@
   <dimension ref="A1:O44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A13" sqref="A13:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,7 +1133,7 @@
     <col min="7" max="7" width="23.7109375" style="23" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="65.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.140625" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" customWidth="1"/>
     <col min="13" max="13" width="12.5703125" customWidth="1"/>
@@ -1046,7 +1142,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1261,30 +1357,30 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="42"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="41"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="36" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="35" t="s">
         <v>64</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1335,178 +1431,178 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="30">
+      <c r="A13" s="29">
         <v>1</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="32">
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="31">
         <v>100</v>
       </c>
-      <c r="G13" s="33">
+      <c r="G13" s="32">
         <v>132855836</v>
       </c>
-      <c r="H13" s="31" t="s">
+      <c r="H13" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="34">
+      <c r="I13" s="33">
         <v>41416</v>
       </c>
-      <c r="J13" s="34" t="s">
+      <c r="J13" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="31" t="s">
+      <c r="K13" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="L13" s="31" t="s">
+      <c r="L13" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M13" s="35" t="s">
+      <c r="M13" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="N13" s="31" t="s">
+      <c r="N13" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="O13" s="34">
+      <c r="O13" s="33">
         <v>41958</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="30">
+      <c r="A14" s="29">
         <v>2</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="31">
         <v>109</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="31" t="s">
+      <c r="H14" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="34">
+      <c r="I14" s="33">
         <v>41416</v>
       </c>
-      <c r="J14" s="34" t="s">
+      <c r="J14" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="31" t="s">
+      <c r="K14" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="L14" s="31" t="s">
+      <c r="L14" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="M14" s="35" t="s">
+      <c r="M14" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="N14" s="31" t="s">
+      <c r="N14" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="O14" s="34">
+      <c r="O14" s="33">
         <v>41991</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="30">
+      <c r="A15" s="29">
         <v>3</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="32">
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31">
         <v>27</v>
       </c>
-      <c r="G15" s="33">
+      <c r="G15" s="32">
         <v>321784073</v>
       </c>
-      <c r="H15" s="31" t="s">
+      <c r="H15" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="I15" s="34">
+      <c r="I15" s="33">
         <v>41416</v>
       </c>
-      <c r="J15" s="34" t="s">
+      <c r="J15" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="K15" s="31" t="s">
+      <c r="K15" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="L15" s="31" t="s">
+      <c r="L15" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="M15" s="35" t="s">
+      <c r="M15" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="N15" s="31" t="s">
+      <c r="N15" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="O15" s="34">
+      <c r="O15" s="33">
         <v>41654</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="30">
+      <c r="A16" s="29">
         <v>4</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32">
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31">
         <v>34</v>
       </c>
-      <c r="G16" s="33">
+      <c r="G16" s="32">
         <v>1449319270</v>
       </c>
-      <c r="H16" s="31" t="s">
+      <c r="H16" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="I16" s="34">
+      <c r="I16" s="33">
         <v>41416</v>
       </c>
-      <c r="J16" s="34" t="s">
+      <c r="J16" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="K16" s="31" t="s">
+      <c r="K16" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="L16" s="31" t="s">
+      <c r="L16" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="M16" s="35" t="s">
+      <c r="M16" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="N16" s="31" t="s">
+      <c r="N16" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="O16" s="34">
+      <c r="O16" s="33">
         <v>41867</v>
       </c>
     </row>
@@ -1709,125 +1805,142 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" style="28" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="38" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C4" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="28">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="29">
         <v>1</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C5" s="29">
         <v>1</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D5" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19" t="s">
+      <c r="E5" s="30"/>
+      <c r="F5" s="30" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="28">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="29">
         <v>1</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C6" s="29">
         <v>2</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D6" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19" t="s">
+      <c r="E6" s="30"/>
+      <c r="F6" s="30" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="28">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="29">
         <v>2</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C7" s="29">
         <v>2</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D7" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19" t="s">
+      <c r="E7" s="30"/>
+      <c r="F7" s="30" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="28">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="29">
         <v>3</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C8" s="29">
         <v>4</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D8" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E8" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F8" s="30" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="28">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="29">
         <v>4</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C9" s="29">
         <v>3</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D9" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19" t="s">
+      <c r="E9" s="30"/>
+      <c r="F9" s="30" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="28">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="29">
         <v>5</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C10" s="29">
         <v>2</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D10" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19" t="s">
+      <c r="E10" s="30"/>
+      <c r="F10" s="30" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1839,36 +1952,371 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="38" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="29">
+        <v>1</v>
+      </c>
+      <c r="C5" s="29">
+        <v>1</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="31">
+        <v>100</v>
+      </c>
+      <c r="F5" s="32">
+        <v>132855836</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="29">
+        <v>2</v>
+      </c>
+      <c r="C6" s="29">
+        <v>1</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="31">
+        <v>109</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="29">
+        <v>2</v>
+      </c>
+      <c r="C7" s="29">
+        <v>2</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="31">
+        <v>109</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="29">
+        <v>2</v>
+      </c>
+      <c r="C8" s="29">
+        <v>5</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="31">
+        <v>109</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="29">
+        <v>3</v>
+      </c>
+      <c r="C9" s="29">
+        <v>4</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="31">
+        <v>27</v>
+      </c>
+      <c r="F9" s="32">
+        <v>321784073</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="29">
+        <v>4</v>
+      </c>
+      <c r="C10" s="29">
+        <v>3</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="31">
+        <v>34</v>
+      </c>
+      <c r="F10" s="32">
+        <v>1449319270</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E15CAA-4777-4BDE-A5C1-09049BF5293E}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="64.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="48">
+        <v>1</v>
+      </c>
+      <c r="C5" s="29">
+        <v>1</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="33">
+        <v>41416</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="48">
+        <v>2</v>
+      </c>
+      <c r="C6" s="29">
+        <v>3</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="33">
+        <v>41416</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="48">
+        <v>3</v>
+      </c>
+      <c r="C7" s="29">
+        <v>2</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="33">
+        <v>41416</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="48">
+        <v>4</v>
+      </c>
+      <c r="C8" s="29">
+        <v>1</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="33">
+        <v>41416</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="48">
+        <v>5</v>
+      </c>
+      <c r="C9" s="29">
+        <v>2</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" s="33">
+        <v>41416</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="48">
+        <v>6</v>
+      </c>
+      <c r="C10" s="29">
+        <v>4</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="33">
+        <v>41416</v>
+      </c>
+      <c r="F10" s="33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="48">
+        <v>7</v>
+      </c>
+      <c r="C11" s="29">
+        <v>4</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="33">
+        <v>41416</v>
+      </c>
+      <c r="F11" s="33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="48">
+        <v>8</v>
+      </c>
+      <c r="C12" s="29">
+        <v>2</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="33">
+        <v>41416</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B5:F12">
+    <sortCondition ref="D5:D12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A6F80E-60BB-4B9E-9A06-656EDAEA79F7}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="37" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Completed Final PROG1500
</commit_message>
<xml_diff>
--- a/Courses/PROG1500 - Databases and SQL/Modules/Final Project/Final_Project.xlsx
+++ b/Courses/PROG1500 - Databases and SQL/Modules/Final Project/Final_Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4400113921\Desktop\Ryan\Software_Technology\Courses\PROG1500 - Databases and SQL\Modules\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900D97C7-7D25-42D3-9B1B-2CB662E7EA41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DFC2E1-6532-4F7A-A8DA-5C1791679122}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15480" windowHeight="9645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15480" windowHeight="9645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fake Online Bookstore dataset" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="126">
   <si>
     <t>PK</t>
   </si>
@@ -351,6 +351,57 @@
   </si>
   <si>
     <t>"Its the book you need if you want to learn HTML"</t>
+  </si>
+  <si>
+    <t>customer_id</t>
+  </si>
+  <si>
+    <t>Gill</t>
+  </si>
+  <si>
+    <t>Bennett</t>
+  </si>
+  <si>
+    <t>Gomez</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>middle_initial</t>
+  </si>
+  <si>
+    <t>C.</t>
+  </si>
+  <si>
+    <t>A.</t>
+  </si>
+  <si>
+    <t>S.</t>
+  </si>
+  <si>
+    <t>L.</t>
+  </si>
+  <si>
+    <t>Terry</t>
+  </si>
+  <si>
+    <t>Johnathan</t>
+  </si>
+  <si>
+    <t>Kathryn</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>adddress</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
@@ -1119,8 +1170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,8 +1184,8 @@
     <col min="7" max="7" width="23.7109375" style="23" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="65.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" customWidth="1"/>
     <col min="13" max="13" width="12.5703125" customWidth="1"/>
     <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -1808,14 +1859,17 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1962,7 +2016,7 @@
   <cols>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2109,20 +2163,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E15CAA-4777-4BDE-A5C1-09049BF5293E}">
   <dimension ref="B1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>91</v>
       </c>
       <c r="D1" s="9"/>
@@ -2302,21 +2357,187 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A6F80E-60BB-4B9E-9A06-656EDAEA79F7}">
-  <dimension ref="B1:B2"/>
+  <dimension ref="B1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="37" t="s">
+    <row r="1" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="38" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="2:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="29">
+        <v>1</v>
+      </c>
+      <c r="C5" s="29">
+        <v>2</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="33">
+        <v>41991</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="29">
+        <v>2</v>
+      </c>
+      <c r="C6" s="29">
+        <v>1</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="H6" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="33">
+        <v>41958</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="29">
+        <v>3</v>
+      </c>
+      <c r="C7" s="29">
+        <v>3</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="33">
+        <v>41654</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="29">
+        <v>4</v>
+      </c>
+      <c r="C8" s="29">
+        <v>4</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="33">
+        <v>41867</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="C5:J8">
+    <sortCondition ref="G5:G8"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>